<commit_message>
Major update: Added Patient Intake form with Excel integration, collapsible timeline tiles, and dose level selection
- Added comprehensive Patient Intake tab with full patient information form
- Integrated intake form to save directly to Excel file (Dashboard Clone.xlsx Active tab)
- Implemented collapsible patient timeline tiles with proper spacing
- Added Regular Dose/High Dose selection field to intake form
- Created inline editing for patient details modal
- Replaced Area with City throughout the application
- Added Doula field and removed Chaplain field
- Changed Admission Date to Intake Date
- Replaced multiple insurance fields with single Medi-Cal ID Number field
- Fixed duplicate patient entry issues and added alphabetical sorting
- Added API endpoint for saving patient data to Excel
- Enhanced UI with better patient detail views and timeline functionality
- Fixed date input validation issues for MM/DD/YYYY format
</commit_message>
<xml_diff>
--- a/Dashboard Clone.xlsx
+++ b/Dashboard Clone.xlsx
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AH11"/>
+  <dimension ref="A1:AJ13"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1547,9 +1547,220 @@
         <v>Peaceful End</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Test Patient Excel</v>
+      </c>
+      <c r="B12" t="str">
+        <v>65</v>
+      </c>
+      <c r="C12" t="str">
+        <v>San Diego</v>
+      </c>
+      <c r="D12" t="str">
+        <v>Dr. Test Doctor</v>
+      </c>
+      <c r="E12" t="str">
+        <v>Test Hospice</v>
+      </c>
+      <c r="F12" t="str">
+        <v>Test Diagnosis</v>
+      </c>
+      <c r="G12" t="str">
+        <v>12/15/2024</v>
+      </c>
+      <c r="H12" t="str">
+        <v>(555) 123-4567</v>
+      </c>
+      <c r="I12" t="str">
+        <v>test@example.com</v>
+      </c>
+      <c r="J12" t="str">
+        <v>no</v>
+      </c>
+      <c r="K12" t="str">
+        <v/>
+      </c>
+      <c r="L12" t="str">
+        <v>03/15/1959</v>
+      </c>
+      <c r="M12" t="str">
+        <v>12/15/2024</v>
+      </c>
+      <c r="N12" t="str">
+        <v>1500.00</v>
+      </c>
+      <c r="O12" t="str">
+        <v>MC987654321</v>
+      </c>
+      <c r="P12" t="str">
+        <v>Regular Dose</v>
+      </c>
+      <c r="Q12" t="str">
+        <v>456 Test Street</v>
+      </c>
+      <c r="R12" t="str">
+        <v>CA</v>
+      </c>
+      <c r="S12" t="str">
+        <v>92101</v>
+      </c>
+      <c r="T12" t="str">
+        <v>Test Contact</v>
+      </c>
+      <c r="U12" t="str">
+        <v>(555) 987-6543</v>
+      </c>
+      <c r="V12" t="str">
+        <v>Spouse</v>
+      </c>
+      <c r="W12" t="str">
+        <v>Secondary Test</v>
+      </c>
+      <c r="X12" t="str">
+        <v>Test symptoms</v>
+      </c>
+      <c r="Y12" t="str">
+        <v>Test medical history</v>
+      </c>
+      <c r="Z12" t="str">
+        <v>Test medications</v>
+      </c>
+      <c r="AA12" t="str">
+        <v>None</v>
+      </c>
+      <c r="AB12" t="str">
+        <v>Less than 6 months</v>
+      </c>
+      <c r="AC12" t="str">
+        <v>Dr. Referring</v>
+      </c>
+      <c r="AD12" t="str">
+        <v>Nurse Test</v>
+      </c>
+      <c r="AE12" t="str">
+        <v>Worker Test</v>
+      </c>
+      <c r="AF12" t="str">
+        <v>Doula Test</v>
+      </c>
+      <c r="AG12" t="str">
+        <v>Standard</v>
+      </c>
+      <c r="AH12" t="str">
+        <v>Test special needs</v>
+      </c>
+      <c r="AI12" t="str">
+        <v>Test notes from Excel integration</v>
+      </c>
+      <c r="AJ12" t="str">
+        <v>Test Staff</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v/>
+      </c>
+      <c r="B13" t="str">
+        <v>8/26/2025</v>
+      </c>
+      <c r="C13" t="str">
+        <v>Test Patient Excel</v>
+      </c>
+      <c r="D13" t="str">
+        <v>03/15/1959</v>
+      </c>
+      <c r="E13" t="str">
+        <v>65</v>
+      </c>
+      <c r="F13" t="str">
+        <v>San Diego</v>
+      </c>
+      <c r="G13" t="str">
+        <v>(555) 123-4567</v>
+      </c>
+      <c r="H13" t="str">
+        <v>test@example.com</v>
+      </c>
+      <c r="I13" t="str">
+        <v/>
+      </c>
+      <c r="J13" t="str">
+        <v/>
+      </c>
+      <c r="K13" t="str">
+        <v>Dr. Test Doctor</v>
+      </c>
+      <c r="L13" t="str">
+        <v/>
+      </c>
+      <c r="M13" t="str">
+        <v/>
+      </c>
+      <c r="N13" t="str">
+        <v/>
+      </c>
+      <c r="O13" t="str">
+        <v>Test Hospice</v>
+      </c>
+      <c r="P13" t="str">
+        <v/>
+      </c>
+      <c r="Q13" t="str">
+        <v/>
+      </c>
+      <c r="R13" t="str">
+        <v>1500.00</v>
+      </c>
+      <c r="S13" t="str">
+        <v>no</v>
+      </c>
+      <c r="T13" t="str">
+        <v/>
+      </c>
+      <c r="U13" t="str">
+        <v>12/15/2024</v>
+      </c>
+      <c r="V13" t="str">
+        <v/>
+      </c>
+      <c r="W13" t="str">
+        <v/>
+      </c>
+      <c r="X13" t="str">
+        <v/>
+      </c>
+      <c r="Y13" t="str">
+        <v/>
+      </c>
+      <c r="Z13" t="str">
+        <v/>
+      </c>
+      <c r="AA13" t="str">
+        <v/>
+      </c>
+      <c r="AB13" t="str">
+        <v/>
+      </c>
+      <c r="AC13" t="str">
+        <v/>
+      </c>
+      <c r="AD13" t="str">
+        <v/>
+      </c>
+      <c r="AE13" t="str">
+        <v/>
+      </c>
+      <c r="AF13" t="str">
+        <v/>
+      </c>
+      <c r="AG13" t="str">
+        <v>Dr. Referring</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AH11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AJ13"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Fix statistics display - show actual numbers instead of template literals
</commit_message>
<xml_diff>
--- a/Dashboard Clone.xlsx
+++ b/Dashboard Clone.xlsx
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ13"/>
+  <dimension ref="A1:AJ14"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1758,9 +1758,110 @@
         <v>Dr. Referring</v>
       </c>
     </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v/>
+      </c>
+      <c r="B14" t="str">
+        <v>9/1/2025</v>
+      </c>
+      <c r="C14" t="str">
+        <v>Sarah Johnson</v>
+      </c>
+      <c r="D14" t="str">
+        <v>05/15/1968</v>
+      </c>
+      <c r="E14" t="str">
+        <v>55</v>
+      </c>
+      <c r="F14" t="str">
+        <v>San Diego</v>
+      </c>
+      <c r="G14" t="str">
+        <v>(619) 555-0123</v>
+      </c>
+      <c r="H14" t="str">
+        <v>sarah.johnson@email.com</v>
+      </c>
+      <c r="I14" t="str">
+        <v/>
+      </c>
+      <c r="J14" t="str">
+        <v/>
+      </c>
+      <c r="K14" t="str">
+        <v>Dr. Emily Rodriguez</v>
+      </c>
+      <c r="L14" t="str">
+        <v/>
+      </c>
+      <c r="M14" t="str">
+        <v/>
+      </c>
+      <c r="N14" t="str">
+        <v/>
+      </c>
+      <c r="O14" t="str">
+        <v>Hospice of San Diego</v>
+      </c>
+      <c r="P14" t="str">
+        <v/>
+      </c>
+      <c r="Q14" t="str">
+        <v/>
+      </c>
+      <c r="R14" t="str">
+        <v>2500.00</v>
+      </c>
+      <c r="S14" t="str">
+        <v>no</v>
+      </c>
+      <c r="T14" t="str">
+        <v/>
+      </c>
+      <c r="U14" t="str">
+        <v>01/15/2024</v>
+      </c>
+      <c r="V14" t="str">
+        <v/>
+      </c>
+      <c r="W14" t="str">
+        <v/>
+      </c>
+      <c r="X14" t="str">
+        <v/>
+      </c>
+      <c r="Y14" t="str">
+        <v/>
+      </c>
+      <c r="Z14" t="str">
+        <v/>
+      </c>
+      <c r="AA14" t="str">
+        <v/>
+      </c>
+      <c r="AB14" t="str">
+        <v/>
+      </c>
+      <c r="AC14" t="str">
+        <v/>
+      </c>
+      <c r="AD14" t="str">
+        <v/>
+      </c>
+      <c r="AE14" t="str">
+        <v/>
+      </c>
+      <c r="AF14" t="str">
+        <v/>
+      </c>
+      <c r="AG14" t="str">
+        <v>Dr. James Wilson</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AJ13"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AJ14"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
Update dashboard with latest changes
- Updated Excel file with new patient data
- Fixed task status colors and persistence
- Consolidated CSS styles for better performance
- Added debugging for task status updates
- Dashboard is now fully functional with proper color indicators
</commit_message>
<xml_diff>
--- a/Dashboard Clone.xlsx
+++ b/Dashboard Clone.xlsx
@@ -404,7 +404,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AJ14"/>
+  <dimension ref="A1:AJ15"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -1859,9 +1859,110 @@
         <v>Dr. James Wilson</v>
       </c>
     </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v/>
+      </c>
+      <c r="B15" t="str">
+        <v>9/4/2025</v>
+      </c>
+      <c r="C15" t="str">
+        <v>Sarah Johnson</v>
+      </c>
+      <c r="D15" t="str">
+        <v>05/15/1968</v>
+      </c>
+      <c r="E15" t="str">
+        <v>55</v>
+      </c>
+      <c r="F15" t="str">
+        <v>San Diego</v>
+      </c>
+      <c r="G15" t="str">
+        <v>(619) 555-0123</v>
+      </c>
+      <c r="H15" t="str">
+        <v>sarah.johnson@email.com</v>
+      </c>
+      <c r="I15" t="str">
+        <v/>
+      </c>
+      <c r="J15" t="str">
+        <v/>
+      </c>
+      <c r="K15" t="str">
+        <v>Dr. Emily Rodriguez</v>
+      </c>
+      <c r="L15" t="str">
+        <v/>
+      </c>
+      <c r="M15" t="str">
+        <v/>
+      </c>
+      <c r="N15" t="str">
+        <v/>
+      </c>
+      <c r="O15" t="str">
+        <v>Hospice of San Diego</v>
+      </c>
+      <c r="P15" t="str">
+        <v/>
+      </c>
+      <c r="Q15" t="str">
+        <v/>
+      </c>
+      <c r="R15" t="str">
+        <v>2500.00</v>
+      </c>
+      <c r="S15" t="str">
+        <v>no</v>
+      </c>
+      <c r="T15" t="str">
+        <v/>
+      </c>
+      <c r="U15" t="str">
+        <v>01/15/2024</v>
+      </c>
+      <c r="V15" t="str">
+        <v/>
+      </c>
+      <c r="W15" t="str">
+        <v/>
+      </c>
+      <c r="X15" t="str">
+        <v/>
+      </c>
+      <c r="Y15" t="str">
+        <v/>
+      </c>
+      <c r="Z15" t="str">
+        <v/>
+      </c>
+      <c r="AA15" t="str">
+        <v/>
+      </c>
+      <c r="AB15" t="str">
+        <v/>
+      </c>
+      <c r="AC15" t="str">
+        <v/>
+      </c>
+      <c r="AD15" t="str">
+        <v/>
+      </c>
+      <c r="AE15" t="str">
+        <v/>
+      </c>
+      <c r="AF15" t="str">
+        <v/>
+      </c>
+      <c r="AG15" t="str">
+        <v>Dr. James Wilson</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:AJ14"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:AJ15"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>